<commit_message>
refact : CropCategory 추가
</commit_message>
<xml_diff>
--- a/src/main/resources/init-data/crop_final.xlsx
+++ b/src/main/resources/init-data/crop_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ynuo365-my.sharepoint.com/personal/22010668_ynu_kr/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimdoyeon/Desktop/NYM/src/main/resources/init-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5B7D02A-C2C8-6242-9F84-AE4AA66F47EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF0D865-5E8A-544C-A1A4-FE403833AD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="5480" windowWidth="38400" windowHeight="21620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="576">
   <si>
     <t>카테고리</t>
   </si>
@@ -1472,261 +1472,6 @@
     <t>회향풀 또는 그 열매를 말하며 대회향과 소회향이 있는데 약으로도 쓰고 기름도 짬.</t>
   </si>
   <si>
-    <t>잡초</t>
-  </si>
-  <si>
-    <t>가는보리풀</t>
-  </si>
-  <si>
-    <t>가는살갈퀴</t>
-  </si>
-  <si>
-    <t>가는털비름</t>
-  </si>
-  <si>
-    <t>가락지나물</t>
-  </si>
-  <si>
-    <t>166</t>
-  </si>
-  <si>
-    <t>장미과에 속하는 다년초. 줄기는 땅으로 뻗고, 길이 60㎝ 가량이며, 근생엽(根生葉)은 장병(長柄)으로 다섯 개의 소엽(小葉)이 있고, 거친 톱니로 둘렸음. 뱀혀. 학명은 Potentilla anemonifolia Lehm.</t>
-  </si>
-  <si>
-    <t>가래</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>떡이나 엿 따위를 둥글고 길게 늘어놓은 토막.</t>
-  </si>
-  <si>
-    <t>가막사리</t>
-  </si>
-  <si>
-    <t>245</t>
-  </si>
-  <si>
-    <t>국화과에 속하는 일년생 풀로 앞은 보통 세 갈래로 갈라지고 습지에서 나며, 꽃은 황색이며 가을에 핌. 학명은 Bidens tripartita L.</t>
-  </si>
-  <si>
-    <t>가시박</t>
-  </si>
-  <si>
-    <t>가시비름</t>
-  </si>
-  <si>
-    <t>가시상추</t>
-  </si>
-  <si>
-    <t>가을강아지풀</t>
-  </si>
-  <si>
-    <t>갈대</t>
-  </si>
-  <si>
-    <t>1173</t>
-  </si>
-  <si>
-    <t>화본과에 속하는 다년생으로서 습지나 물가에 자생하는 야초. 학명은 Phragmites australis</t>
-  </si>
-  <si>
-    <t>갈퀴꼭두서니</t>
-  </si>
-  <si>
-    <t>갈퀴나물</t>
-  </si>
-  <si>
-    <t>갈퀴덩굴</t>
-  </si>
-  <si>
-    <t>1267</t>
-  </si>
-  <si>
-    <t>꼭두서닛과에 속하는 이년생(二年生) 만초(萬草). 줄기 길이 1m 가량이며 잎은 피침형으로 가늘고 긴데 대개 6∼8개씩 윤생(輪生)함. 학명은 Galium spurium var. echinospermon</t>
-  </si>
-  <si>
-    <t>강아지풀</t>
-  </si>
-  <si>
-    <t>1705</t>
-  </si>
-  <si>
-    <t>볏과에 속(屬)하는 일년초. 줄기는 총생(叢生)하고 높이 30∼70cm 이며, 잎은 선형(線形) 또는 피침형 선상(線狀)이고 호생함.</t>
-  </si>
-  <si>
-    <t>강피</t>
-  </si>
-  <si>
-    <t>1807</t>
-  </si>
-  <si>
-    <t>포아풀과(벼과)에 속한 1년초. 논에 발생하는데 줄기는 편형, 직진, 평활하며 약 1m가량. 뿌리는 수염모양으로 생겼으며 잎은 길어 피침형이고 8∼9월에 담록색의 꽃이 됨.</t>
-  </si>
-  <si>
-    <t>개갓냉이</t>
-  </si>
-  <si>
-    <t>개구리미나리</t>
-  </si>
-  <si>
-    <t>개구리밥</t>
-  </si>
-  <si>
-    <t>1867</t>
-  </si>
-  <si>
-    <t>개구리밥과에 속하는 다년생 수초(水草). 수면에 뜨며 늦가을에 타원형의 동아(冬芽)가 모체에서 떨어져 나와 물 밑에서 월동하고, 이듬해 봄에 수면에 떠서 번식함. 학명은 Spirodela polyrhiza</t>
-  </si>
-  <si>
-    <t>개기장</t>
-  </si>
-  <si>
-    <t>1879</t>
-  </si>
-  <si>
-    <t>벼과의 1년생초로 숲가나 들에 자라며, 원기둥형의 가는 줄기가 곧게 자라고 키는 30∼120cm이며 가지를 많이 침. 학명은 Panicum bisulcatum Thunb.</t>
-  </si>
-  <si>
-    <t>개꽃아재비</t>
-  </si>
-  <si>
-    <t>개망초</t>
-  </si>
-  <si>
-    <t>개미자리</t>
-  </si>
-  <si>
-    <t>1945</t>
-  </si>
-  <si>
-    <t>석죽과(石竹科)에 속하는 풀. 작은 풀로서 잎은 좁고 광택이 있으며 흰 꽃이 핌. 학명은 Sagina japonica (Sw.) Ohwi</t>
-  </si>
-  <si>
-    <t>개밀</t>
-  </si>
-  <si>
-    <t>1952</t>
-  </si>
-  <si>
-    <t>벼과에 속하는 월년생 식물. 밀과 비슷하나 줄기와 잎은 적갈색이고 줄기는 가늘고 들이나 길가에 나는데 한국, 일본, 중국 등에 분포함.</t>
-  </si>
-  <si>
-    <t>개보리</t>
-  </si>
-  <si>
-    <t>개불알풀</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>현삼과의 두해살이풀. 줄기는 높이가 5~15cm이며, 부드러운 잔털이 많이 나 있다. 잎은 아래쪽에서는 마주나고 위쪽에서는 어긋난다. 5~6월에 엷은 붉은 보라색 꽃이 하나씩 피고 열매는 개 불알 모양의 삭과(蒴果)로 잎겨드랑이에 하나씩 달린다. 들이나 논밭에 나는데 우리나라 중ㆍ남부 지방에 널리 분포한다. 학명은 Veronica didyma var. lilacina</t>
-  </si>
-  <si>
-    <t>개비름</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>비름과에 속하는 일년생 풀의 하나. 줄기는 연질이고 잎은 호생하며 달걀모양임. 논밭이나 길가에 많이 분포하고 어린잎은 식용함.</t>
-  </si>
-  <si>
-    <t>개소시랑개비</t>
-  </si>
-  <si>
-    <t>개쇠뜨기</t>
-  </si>
-  <si>
-    <t>개쑥갓</t>
-  </si>
-  <si>
-    <t>개여뀌</t>
-  </si>
-  <si>
-    <t>개자리</t>
-  </si>
-  <si>
-    <t>2090</t>
-  </si>
-  <si>
-    <t>개질경이</t>
-  </si>
-  <si>
-    <t>개피</t>
-  </si>
-  <si>
-    <t>갯드렁새</t>
-  </si>
-  <si>
-    <t>갯메꽃</t>
-  </si>
-  <si>
-    <t>갯줄풀</t>
-  </si>
-  <si>
-    <t>거지덩굴</t>
-  </si>
-  <si>
-    <t>2388</t>
-  </si>
-  <si>
-    <t>포도과에 속하는 다년생 만초(蔓草). 지하경(地下莖)은 땅 속에 가로 뻗으며 줄기는 모가나고 녹자색으로 다른 것에 감기어 올라감.</t>
-  </si>
-  <si>
-    <t>겨우사리</t>
-  </si>
-  <si>
-    <t>겹달맞이꽃</t>
-  </si>
-  <si>
-    <t>계요등</t>
-  </si>
-  <si>
-    <t>고들빼기</t>
-  </si>
-  <si>
-    <t>108987</t>
-  </si>
-  <si>
-    <t>국화과에 속하는 2년생 초본식물이다. 우리나라 중부 이남에 분포하며 산기슭, 들, 밭두둑, 길가에 자생한다. 키는 80cm 정도이며 줄기는 적자색을 띤다. 뿌리 부근에서 나는 잎은 털이 없고 타원형이며 잎의 가장자리가 빗살처럼 갈라져 있으며 잎자루는 없고 잎의 앞면은 녹색이며 뒷면은 회청색이다. 줄기에 나는 잎은 난형이고 밑이 넓어져서 줄기를 감싼다. 잎에는 불규칙한 톱니가 있으며 위쪽으로 갈수록 작아진다.</t>
-  </si>
-  <si>
-    <t>고마리</t>
-  </si>
-  <si>
-    <t>고사리</t>
-  </si>
-  <si>
-    <t>116688</t>
-  </si>
-  <si>
-    <t>참고사리과에 속하는 다년생의 양치류(羊齒類)로 햇빛이 잘 쬐는 산야에서 자생하는 구황식품이다. 근경(根莖)은 연필대만큼 크고 굳으며 땅 속에서 가로누워 있다. 이른 봄에 싹이 근경에서 돋아 나와서 꼭대기가 꼬불꼬불하게 말리고 흰 솜 같은 털로 온통 덮여 있다. 어린 잎과 줄기를 채취하여 삶은 다음 물에 담구어 식물의 쓴맛과 떫은 맛을 우려낸 후 건조하여 저장한다.</t>
-  </si>
-  <si>
-    <t>고삼</t>
-  </si>
-  <si>
-    <t>176628</t>
-  </si>
-  <si>
-    <t>콩과의 여러해살이풀. 높이는 80~100cm이며, 여름에 나비 모양의 엷은 노란색 꽃이 총상(總狀) 화서로 줄기와 가지 끝에 핀다. 협과(莢果)를 맺으며 뿌리는 약용한다. 산이나 들에서 나는데 우리나라 각지에 분포한다.</t>
-  </si>
-  <si>
-    <t>골풀</t>
-  </si>
-  <si>
-    <t>5241</t>
-  </si>
-  <si>
-    <t>골풀과의 여러해살이풀. 높이는 1미터 정도이고 땅속줄기는 옆으로 뻗으며, 잎은 줄기 아랫부분에 비늘 모양으로 붙어 있다. 5~6월에 녹빛을 띤 노란색 꽃이 취산(聚繖) 화서로 줄기 끝에 피고, 열매는 삭과(蒴果)를 맺는다. 말린 줄기는 약재(藥材)나 자리를 만드는 데 쓴다. 들의 물가나 습한 땅에서 자라는데 한국, 일본, 중국 등지에 분포한다.</t>
-  </si>
-  <si>
-    <t>공단풀</t>
-  </si>
-  <si>
     <t>벼목 벼과에 속하는 한해살이풀이자 곡류의 일종.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1951,14 +1696,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>열대아시아에서 유래한 귀화식물로서 한해살이풀이다. 키는 30~70cm이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>고마리는 마디풀과에 딸린 한해살이풀이다. 한국 원산이며 중국·일본·러시아 극동부에도 서식한다. 메밀 비슷한 열매가 맺는데, 그것으로 수제비 비슷한 음식을 만들어 먹기 위해 구황식물로 재배되었던 적도 있으나, 지금은 잡초이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>꽃자루가 긴 화려한 꽃을 피우는 난초과의 관엽식물</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2095,123 +1832,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>계요등(鷄尿藤)은 꼭두서니과의 잎 지는 덩굴나무이다. 아시아 온대와 열대 전역에 분포한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>달맞이꽃속은 바늘꽃과의 속으로 약 125 종으로 이루어져 있다. 원산지는 칠레이며 7월에 노란 꽃이 핀다. 밤에만 꽃이 피기 때문에 ‘달맞이꽃’, ‘월견초’라 한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>쌍떡잎식물 단향목에 속하는 기생 식물들을 일컫는 말. 기생관목. 겨우살이, 겨우사리, 동청(冬靑), 기생목(寄生木) 등으로 불린다. 영어로는 Mistletoe라고 한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>여러해살이풀로 갯벌 조간대에서 자라며, 땅속줄기가 길게 벋고 마디에서 줄기를 내어 큰 군락을 이룬다. 어른 키보다 높게 자라고 굵기는 0.5-1.5cm이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">갯메꽃(Calystegia soldanella)은 여러해살이 덩굴식물로서[1], 땅속 줄기는 모래 속에 길게 뻗고, 땅위줄기는 땅 위에 가로눕거나 다른 물건에 감겨서 뻗는다. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>갯드렁새속(----屬, 학명: Diplachne 디플라크네[*])은 벼과의 속이다.[1] 과거에는 100여 종을 포함하는 큰 속으로 여겨졌으나, 많은 종이 다른 속으로 재분류되었다. 갯드렁새속에 속하는 2종 중 갯드렁새 1종이 한국에 자생한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개피는 벼과 개피속의 두해살이풀로 학명은 Beckmannia syzigachne이다. 늪피 또는 물피라고도 한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개질경이(Plantago camtschatica)는 한국 각처의 해변이나 들에 나는 여러해살이풀이다. 전체에 거친 털이 밀생하며 원줄기는 없다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개자리속은 콩과의 여러해살이풀로 이루어진 속이다. 종에 따라 알팔파(스페인어: alfalfa), 루선(lucerne)이라고도 부른다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개여뀌는 마디풀과 여뀌속의 한해살이풀이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개쑥갓(Senecio vulgaris)은 국화과에 딸린 한해살이풀길가나 빈터에서 흔하게 자란다. 유럽 원산의 귀화식물이며, 거의 1년 내내 꽃이 핀다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개소시랑개비(문화어: 깃쇠스랑개비)는 앵초과에 속하는 여러해살이풀이다. 북부 아프리카, 유라시아 원산이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>물가에 자라는 여러해살이풀이다. 지상경은 생식줄기만 있으며, 높이 20-80cm, 직경 2-5mm, 5-10개의 능선이 있고 가지는 10개 미만으로 달리며, 끝 부분에는 가지가 없다. 잎집은 길이 4-12mm, 연한 녹색이다. 치편의 끝은 진한 갈색이며, 길이 1.2-4.0mm, 가장자리는 흰색의 막질이다. 포자낭이삭은 원줄기 끝에 붙으며, 타원형, 길이 1-3cm이다. 우리나라 북부지방에 자라며, 울릉도와 대구 등지에서 채집된 기록이 있으나, 더 이상 확인되고 있지 않고 있다. 세계적으로 북반구 온대의 북부지방에 분포한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개보리는 벼과의 여러해살이풀로 학명은 Elymus sibiricus이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개망초(영어: annual fleabane, daisy fleabane 또는 eastern daisy fleabane)는 전 세계 온대 지방에 주로 서식하는 국화과의 두해살이풀이다. 망국초, 왜풀, 개망풀이라고도 한다.[1] 북아메리카 원산의 귀화식물이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>햇볕이 잘 드는 공한지, 길가 등에 자라는 한해살이풀로 귀화식물이다. 줄기는 높이 20~40cm이다. 잎은 어긋나며, 대개는 잎자루가 없다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개구리미나리(Ranunculus tachiroei)는 한국 각처 산이나 들의 습지에 나는 두해살이풀이다. 길이는 50-100cm이다. 근생엽과 밑부분의 경생엽은 잎자루가 길고, 2회 3출의 작은잎으로 된 겹잎, 작은잎은 길이 3-6cm, 깊게 2-3갈래, 가장자리에 불규칙한 톱니 모양이다. 꽃은 취산꽃차례로 노란색이며 지름 1cm 내외이다. 꽃받침은 5장, 연녹색, 겉에 털이 약간 있다. 열매는 수과로 화탁에 모여 별사탕 모양의 열매 덩이를 형성한다. 줄기와 잎은 약용으로 쓴다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>민가 주변 길가, 경작지 및 산지 숲 가장자리의 햇빛이 잘 드는 곳에 자라는 여러해살이풀이다. 줄기는 높이 20~50cm, 가지가 많이 갈라지며, 전체에 털이 없다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>갈퀴나물은 한국을 비롯하여 일본·중국·시베리아의 온대에서 난대에 걸쳐 분포하는 여러해살이 덩굴식물로 들에서 자란다. 땅속줄기를뻗으면서 자라며 줄기는 길이 1-2m로 능선이 있어 네모진다. 잎은 어긋나며 거의 잎자루가 없다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>쌍떡잎식물 꿀풀목 꿀풀과 골무꽃속에 속하는 식물이자 한방에서 쓰이는 중요 약재. 순우리말로는 '속썩은풀'이라고도 한다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>황기(黃芪/黃耆)는 콩과에 속하는 다년생 초본식물이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>가는 보리풀은 유럽에서 들어온 외래종으로 초장은 30~60㎝이며, 많이 모여 나고 곧추서고, 하부는 흔히 붉은빛을 띠는 것으로 알려져 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주로 들이나 저지대의 햇빛이 잘 드는 풀밭에서 자라는 여러해살이풀이다. 줄기는 높이 60~150cm, 덩굴지거나 다른 물체를 감고 오르며, 단면은 네모나고, 연한 털이 있거나 없다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>가시도꼬마리</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">길가나 들판에 자라는 한해살이풀이다. 줄기는 높이 40~120cm, 전체에 검은 자주색 잔 점이 있다. 잎은 어긋나며 길이 6~12cm의 잎자루가 있다. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>가시박(Sicyos angulatus)은 북미 원산의 박과 식물로 한해살이풀이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>가시비름은 쌍떡잎식물 중심자목 비름과의 한해살이풀이다. 남아메리카가 원산이다. 높이는 40~80cm이고 줄기에 능선이 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>국화과에 속하는 한해살이 혹은 두해살이풀. 한국인이 쌈채소로 즐겨먹는 상추의 야생종이다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>경작지 주변이나 길가에 흔하게 자라는 한해살이풀이다. 줄기는 곧추서거나 밑부분이 휘어지며 높이 40~100cm이다. 잎집의 가장자리에 센털이 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다년초여부: 다년생 - Perennial plant ; 열매. 장과는 2개씩 달리고 둥글며 지름 5-6mm로 8-9월에 흑색으로 익으며 1개의 종자가 들어 있다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2588,10 +2213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E267"/>
+  <dimension ref="A1:E217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="A218" sqref="A218:H269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -2797,7 +2422,7 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>568</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2859,7 +2484,7 @@
         <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>569</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2904,7 +2529,7 @@
         <v>54</v>
       </c>
       <c r="E19" t="s">
-        <v>570</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3051,7 +2676,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>571</v>
+        <v>486</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3085,7 +2710,7 @@
         <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>572</v>
+        <v>487</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3181,7 +2806,7 @@
         <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>573</v>
+        <v>488</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3209,7 +2834,7 @@
         <v>105</v>
       </c>
       <c r="E38" t="s">
-        <v>574</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3288,7 +2913,7 @@
         <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>575</v>
+        <v>490</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3367,7 +2992,7 @@
         <v>132</v>
       </c>
       <c r="E48" t="s">
-        <v>576</v>
+        <v>491</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3701,7 +3326,7 @@
         <v>190</v>
       </c>
       <c r="E68" t="s">
-        <v>577</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3729,7 +3354,7 @@
         <v>194</v>
       </c>
       <c r="E70" t="s">
-        <v>578</v>
+        <v>493</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3825,7 +3450,7 @@
         <v>210</v>
       </c>
       <c r="E76" t="s">
-        <v>579</v>
+        <v>494</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3853,7 +3478,7 @@
         <v>214</v>
       </c>
       <c r="E78" t="s">
-        <v>580</v>
+        <v>495</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3915,7 +3540,7 @@
         <v>224</v>
       </c>
       <c r="E82" t="s">
-        <v>581</v>
+        <v>496</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -3974,10 +3599,10 @@
         <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>582</v>
+        <v>497</v>
       </c>
       <c r="E86" t="s">
-        <v>583</v>
+        <v>498</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -3988,7 +3613,7 @@
         <v>234</v>
       </c>
       <c r="E87" t="s">
-        <v>584</v>
+        <v>499</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3999,7 +3624,7 @@
         <v>235</v>
       </c>
       <c r="E88" t="s">
-        <v>585</v>
+        <v>500</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4027,7 +3652,7 @@
         <v>239</v>
       </c>
       <c r="E90" t="s">
-        <v>586</v>
+        <v>501</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4188,10 +3813,10 @@
         <v>122</v>
       </c>
       <c r="B100" t="s">
-        <v>587</v>
+        <v>502</v>
       </c>
       <c r="E100" t="s">
-        <v>588</v>
+        <v>503</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4270,7 +3895,7 @@
         <v>280</v>
       </c>
       <c r="E105" t="s">
-        <v>589</v>
+        <v>504</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4281,7 +3906,7 @@
         <v>281</v>
       </c>
       <c r="E106" t="s">
-        <v>590</v>
+        <v>505</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4343,7 +3968,7 @@
         <v>291</v>
       </c>
       <c r="E110" t="s">
-        <v>591</v>
+        <v>506</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4371,7 +3996,7 @@
         <v>295</v>
       </c>
       <c r="E112" t="s">
-        <v>592</v>
+        <v>507</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4382,7 +4007,7 @@
         <v>296</v>
       </c>
       <c r="E113" t="s">
-        <v>593</v>
+        <v>508</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4478,7 +4103,7 @@
         <v>309</v>
       </c>
       <c r="E119" t="s">
-        <v>594</v>
+        <v>509</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4540,7 +4165,7 @@
         <v>319</v>
       </c>
       <c r="E123" t="s">
-        <v>690</v>
+        <v>575</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4551,7 +4176,7 @@
         <v>320</v>
       </c>
       <c r="E124" t="s">
-        <v>595</v>
+        <v>510</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4559,10 +4184,10 @@
         <v>267</v>
       </c>
       <c r="B125" t="s">
-        <v>596</v>
+        <v>511</v>
       </c>
       <c r="E125" t="s">
-        <v>597</v>
+        <v>512</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4573,7 +4198,7 @@
         <v>321</v>
       </c>
       <c r="E126" t="s">
-        <v>598</v>
+        <v>513</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4601,7 +4226,7 @@
         <v>325</v>
       </c>
       <c r="E128" t="s">
-        <v>599</v>
+        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4646,7 +4271,7 @@
         <v>332</v>
       </c>
       <c r="E131" t="s">
-        <v>600</v>
+        <v>515</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4671,10 +4296,10 @@
         <v>267</v>
       </c>
       <c r="B133" t="s">
-        <v>601</v>
+        <v>516</v>
       </c>
       <c r="E133" t="s">
-        <v>602</v>
+        <v>517</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4719,7 +4344,7 @@
         <v>342</v>
       </c>
       <c r="E136" t="s">
-        <v>603</v>
+        <v>518</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4761,10 +4386,10 @@
         <v>267</v>
       </c>
       <c r="B139" t="s">
-        <v>604</v>
+        <v>519</v>
       </c>
       <c r="E139" t="s">
-        <v>605</v>
+        <v>520</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -4772,10 +4397,10 @@
         <v>267</v>
       </c>
       <c r="B140" t="s">
-        <v>606</v>
+        <v>521</v>
       </c>
       <c r="E140" t="s">
-        <v>607</v>
+        <v>522</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4817,10 +4442,10 @@
         <v>267</v>
       </c>
       <c r="B143" t="s">
-        <v>608</v>
+        <v>523</v>
       </c>
       <c r="E143" t="s">
-        <v>609</v>
+        <v>524</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -4828,10 +4453,10 @@
         <v>267</v>
       </c>
       <c r="B144" t="s">
-        <v>611</v>
+        <v>526</v>
       </c>
       <c r="E144" t="s">
-        <v>612</v>
+        <v>527</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -4842,7 +4467,7 @@
         <v>355</v>
       </c>
       <c r="E145" t="s">
-        <v>610</v>
+        <v>525</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4850,10 +4475,10 @@
         <v>267</v>
       </c>
       <c r="B146" t="s">
-        <v>614</v>
+        <v>529</v>
       </c>
       <c r="E146" t="s">
-        <v>615</v>
+        <v>530</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -4898,7 +4523,7 @@
         <v>362</v>
       </c>
       <c r="E149" t="s">
-        <v>613</v>
+        <v>528</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -4909,7 +4534,7 @@
         <v>363</v>
       </c>
       <c r="E150" t="s">
-        <v>616</v>
+        <v>531</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -4917,10 +4542,10 @@
         <v>267</v>
       </c>
       <c r="B151" t="s">
-        <v>619</v>
+        <v>534</v>
       </c>
       <c r="E151" t="s">
-        <v>620</v>
+        <v>535</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -4928,10 +4553,10 @@
         <v>267</v>
       </c>
       <c r="B152" t="s">
-        <v>617</v>
+        <v>532</v>
       </c>
       <c r="E152" t="s">
-        <v>618</v>
+        <v>533</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -4939,10 +4564,10 @@
         <v>267</v>
       </c>
       <c r="B153" t="s">
-        <v>621</v>
+        <v>536</v>
       </c>
       <c r="E153" t="s">
-        <v>622</v>
+        <v>537</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -4950,10 +4575,10 @@
         <v>267</v>
       </c>
       <c r="B154" t="s">
-        <v>623</v>
+        <v>538</v>
       </c>
       <c r="E154" t="s">
-        <v>626</v>
+        <v>539</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -4961,10 +4586,10 @@
         <v>267</v>
       </c>
       <c r="B155" t="s">
-        <v>627</v>
+        <v>540</v>
       </c>
       <c r="E155" t="s">
-        <v>628</v>
+        <v>541</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -4992,7 +4617,7 @@
         <v>367</v>
       </c>
       <c r="E157" t="s">
-        <v>629</v>
+        <v>542</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5003,7 +4628,7 @@
         <v>368</v>
       </c>
       <c r="E158" t="s">
-        <v>630</v>
+        <v>543</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5031,7 +4656,7 @@
         <v>372</v>
       </c>
       <c r="E160" t="s">
-        <v>631</v>
+        <v>544</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -5076,7 +4701,7 @@
         <v>379</v>
       </c>
       <c r="E163" t="s">
-        <v>632</v>
+        <v>545</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5206,7 +4831,7 @@
         <v>401</v>
       </c>
       <c r="E171" t="s">
-        <v>633</v>
+        <v>546</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5234,7 +4859,7 @@
         <v>405</v>
       </c>
       <c r="E173" t="s">
-        <v>634</v>
+        <v>547</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5245,7 +4870,7 @@
         <v>406</v>
       </c>
       <c r="E174" t="s">
-        <v>635</v>
+        <v>548</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5256,7 +4881,7 @@
         <v>407</v>
       </c>
       <c r="E175" t="s">
-        <v>636</v>
+        <v>549</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5267,7 +4892,7 @@
         <v>408</v>
       </c>
       <c r="E176" t="s">
-        <v>637</v>
+        <v>550</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5278,7 +4903,7 @@
         <v>409</v>
       </c>
       <c r="E177" t="s">
-        <v>638</v>
+        <v>551</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -5289,7 +4914,7 @@
         <v>410</v>
       </c>
       <c r="E178" t="s">
-        <v>639</v>
+        <v>552</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -5317,7 +4942,7 @@
         <v>415</v>
       </c>
       <c r="E180" t="s">
-        <v>640</v>
+        <v>553</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5325,10 +4950,10 @@
         <v>411</v>
       </c>
       <c r="B181" t="s">
-        <v>641</v>
+        <v>554</v>
       </c>
       <c r="E181" t="s">
-        <v>642</v>
+        <v>555</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5339,7 +4964,7 @@
         <v>416</v>
       </c>
       <c r="E182" t="s">
-        <v>643</v>
+        <v>556</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5486,7 +5111,7 @@
         <v>435</v>
       </c>
       <c r="E191" t="s">
-        <v>644</v>
+        <v>557</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5514,7 +5139,7 @@
         <v>439</v>
       </c>
       <c r="E193" t="s">
-        <v>645</v>
+        <v>558</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -5525,7 +5150,7 @@
         <v>440</v>
       </c>
       <c r="E194" t="s">
-        <v>646</v>
+        <v>559</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -5536,7 +5161,7 @@
         <v>441</v>
       </c>
       <c r="E195" t="s">
-        <v>647</v>
+        <v>560</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -5547,7 +5172,7 @@
         <v>442</v>
       </c>
       <c r="E196" t="s">
-        <v>648</v>
+        <v>561</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5592,7 +5217,7 @@
         <v>449</v>
       </c>
       <c r="E199" t="s">
-        <v>649</v>
+        <v>562</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -5603,7 +5228,7 @@
         <v>450</v>
       </c>
       <c r="E200" t="s">
-        <v>650</v>
+        <v>563</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -5679,10 +5304,10 @@
         <v>411</v>
       </c>
       <c r="B205" t="s">
-        <v>651</v>
+        <v>564</v>
       </c>
       <c r="E205" t="s">
-        <v>652</v>
+        <v>565</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -5744,7 +5369,7 @@
         <v>472</v>
       </c>
       <c r="E209" t="s">
-        <v>653</v>
+        <v>566</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -5755,7 +5380,7 @@
         <v>473</v>
       </c>
       <c r="E210" t="s">
-        <v>654</v>
+        <v>567</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -5763,10 +5388,10 @@
         <v>411</v>
       </c>
       <c r="B211" t="s">
-        <v>656</v>
+        <v>569</v>
       </c>
       <c r="E211" t="s">
-        <v>657</v>
+        <v>570</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -5777,7 +5402,7 @@
         <v>474</v>
       </c>
       <c r="E212" t="s">
-        <v>655</v>
+        <v>568</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -5785,10 +5410,10 @@
         <v>411</v>
       </c>
       <c r="B213" t="s">
-        <v>658</v>
+        <v>571</v>
       </c>
       <c r="E213" t="s">
-        <v>659</v>
+        <v>572</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -5816,7 +5441,7 @@
         <v>478</v>
       </c>
       <c r="E215" t="s">
-        <v>679</v>
+        <v>573</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -5827,7 +5452,7 @@
         <v>479</v>
       </c>
       <c r="E216" t="s">
-        <v>680</v>
+        <v>574</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -5845,673 +5470,6 @@
       </c>
       <c r="E217" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5">
-      <c r="A218" t="s">
-        <v>483</v>
-      </c>
-      <c r="B218" t="s">
-        <v>484</v>
-      </c>
-      <c r="E218" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5">
-      <c r="A219" t="s">
-        <v>483</v>
-      </c>
-      <c r="B219" t="s">
-        <v>485</v>
-      </c>
-      <c r="E219" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5">
-      <c r="A220" t="s">
-        <v>483</v>
-      </c>
-      <c r="B220" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5">
-      <c r="A221" t="s">
-        <v>483</v>
-      </c>
-      <c r="B221" t="s">
-        <v>487</v>
-      </c>
-      <c r="C221">
-        <v>166</v>
-      </c>
-      <c r="D221" t="s">
-        <v>488</v>
-      </c>
-      <c r="E221" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5">
-      <c r="A222" t="s">
-        <v>483</v>
-      </c>
-      <c r="B222" t="s">
-        <v>490</v>
-      </c>
-      <c r="C222">
-        <v>170</v>
-      </c>
-      <c r="D222" t="s">
-        <v>491</v>
-      </c>
-      <c r="E222" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5">
-      <c r="A223" t="s">
-        <v>483</v>
-      </c>
-      <c r="B223" t="s">
-        <v>493</v>
-      </c>
-      <c r="C223">
-        <v>245</v>
-      </c>
-      <c r="D223" t="s">
-        <v>494</v>
-      </c>
-      <c r="E223" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5">
-      <c r="A224" t="s">
-        <v>483</v>
-      </c>
-      <c r="B224" t="s">
-        <v>683</v>
-      </c>
-      <c r="E224" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5">
-      <c r="A225" t="s">
-        <v>483</v>
-      </c>
-      <c r="B225" t="s">
-        <v>496</v>
-      </c>
-      <c r="E225" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5">
-      <c r="A226" t="s">
-        <v>483</v>
-      </c>
-      <c r="B226" t="s">
-        <v>497</v>
-      </c>
-      <c r="E226" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5">
-      <c r="A227" t="s">
-        <v>483</v>
-      </c>
-      <c r="B227" t="s">
-        <v>498</v>
-      </c>
-      <c r="E227" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5">
-      <c r="A228" t="s">
-        <v>483</v>
-      </c>
-      <c r="B228" t="s">
-        <v>499</v>
-      </c>
-      <c r="E228" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5">
-      <c r="A229" t="s">
-        <v>483</v>
-      </c>
-      <c r="B229" t="s">
-        <v>500</v>
-      </c>
-      <c r="C229">
-        <v>1173</v>
-      </c>
-      <c r="D229" t="s">
-        <v>501</v>
-      </c>
-      <c r="E229" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5">
-      <c r="A230" t="s">
-        <v>483</v>
-      </c>
-      <c r="B230" t="s">
-        <v>503</v>
-      </c>
-      <c r="E230" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5">
-      <c r="A231" t="s">
-        <v>483</v>
-      </c>
-      <c r="B231" t="s">
-        <v>504</v>
-      </c>
-      <c r="E231" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5">
-      <c r="A232" t="s">
-        <v>483</v>
-      </c>
-      <c r="B232" t="s">
-        <v>505</v>
-      </c>
-      <c r="C232">
-        <v>1267</v>
-      </c>
-      <c r="D232" t="s">
-        <v>506</v>
-      </c>
-      <c r="E232" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5">
-      <c r="A233" t="s">
-        <v>483</v>
-      </c>
-      <c r="B233" t="s">
-        <v>126</v>
-      </c>
-      <c r="C233">
-        <v>1602</v>
-      </c>
-      <c r="D233" t="s">
-        <v>127</v>
-      </c>
-      <c r="E233" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5">
-      <c r="A234" t="s">
-        <v>483</v>
-      </c>
-      <c r="B234" t="s">
-        <v>508</v>
-      </c>
-      <c r="C234">
-        <v>1705</v>
-      </c>
-      <c r="D234" t="s">
-        <v>509</v>
-      </c>
-      <c r="E234" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5">
-      <c r="A235" t="s">
-        <v>483</v>
-      </c>
-      <c r="B235" t="s">
-        <v>511</v>
-      </c>
-      <c r="C235">
-        <v>1807</v>
-      </c>
-      <c r="D235" t="s">
-        <v>512</v>
-      </c>
-      <c r="E235" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5">
-      <c r="A236" t="s">
-        <v>483</v>
-      </c>
-      <c r="B236" t="s">
-        <v>514</v>
-      </c>
-      <c r="E236" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5">
-      <c r="A237" t="s">
-        <v>483</v>
-      </c>
-      <c r="B237" t="s">
-        <v>515</v>
-      </c>
-      <c r="E237" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5">
-      <c r="A238" t="s">
-        <v>483</v>
-      </c>
-      <c r="B238" t="s">
-        <v>516</v>
-      </c>
-      <c r="C238">
-        <v>1867</v>
-      </c>
-      <c r="D238" t="s">
-        <v>517</v>
-      </c>
-      <c r="E238" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5">
-      <c r="A239" t="s">
-        <v>483</v>
-      </c>
-      <c r="B239" t="s">
-        <v>519</v>
-      </c>
-      <c r="C239">
-        <v>1879</v>
-      </c>
-      <c r="D239" t="s">
-        <v>520</v>
-      </c>
-      <c r="E239" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5">
-      <c r="A240" t="s">
-        <v>483</v>
-      </c>
-      <c r="B240" t="s">
-        <v>522</v>
-      </c>
-      <c r="E240" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5">
-      <c r="A241" t="s">
-        <v>483</v>
-      </c>
-      <c r="B241" t="s">
-        <v>415</v>
-      </c>
-      <c r="E241" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5">
-      <c r="A242" t="s">
-        <v>483</v>
-      </c>
-      <c r="B242" t="s">
-        <v>523</v>
-      </c>
-      <c r="E242" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5">
-      <c r="A243" t="s">
-        <v>483</v>
-      </c>
-      <c r="B243" t="s">
-        <v>524</v>
-      </c>
-      <c r="C243">
-        <v>1945</v>
-      </c>
-      <c r="D243" t="s">
-        <v>525</v>
-      </c>
-      <c r="E243" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5">
-      <c r="A244" t="s">
-        <v>483</v>
-      </c>
-      <c r="B244" t="s">
-        <v>527</v>
-      </c>
-      <c r="C244">
-        <v>1952</v>
-      </c>
-      <c r="D244" t="s">
-        <v>528</v>
-      </c>
-      <c r="E244" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5">
-      <c r="A245" t="s">
-        <v>483</v>
-      </c>
-      <c r="B245" t="s">
-        <v>530</v>
-      </c>
-      <c r="E245" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5">
-      <c r="A246" t="s">
-        <v>483</v>
-      </c>
-      <c r="B246" t="s">
-        <v>531</v>
-      </c>
-      <c r="C246">
-        <v>2022</v>
-      </c>
-      <c r="D246" t="s">
-        <v>532</v>
-      </c>
-      <c r="E246" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="247" spans="1:5">
-      <c r="A247" t="s">
-        <v>483</v>
-      </c>
-      <c r="B247" t="s">
-        <v>534</v>
-      </c>
-      <c r="C247">
-        <v>2023</v>
-      </c>
-      <c r="D247" t="s">
-        <v>535</v>
-      </c>
-      <c r="E247" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="248" spans="1:5">
-      <c r="A248" t="s">
-        <v>483</v>
-      </c>
-      <c r="B248" t="s">
-        <v>537</v>
-      </c>
-      <c r="E248" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="249" spans="1:5">
-      <c r="A249" t="s">
-        <v>483</v>
-      </c>
-      <c r="B249" t="s">
-        <v>538</v>
-      </c>
-      <c r="E249" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="250" spans="1:5">
-      <c r="A250" t="s">
-        <v>483</v>
-      </c>
-      <c r="B250" t="s">
-        <v>539</v>
-      </c>
-      <c r="E250" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="251" spans="1:5">
-      <c r="A251" t="s">
-        <v>483</v>
-      </c>
-      <c r="B251" t="s">
-        <v>540</v>
-      </c>
-      <c r="E251" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="252" spans="1:5">
-      <c r="A252" t="s">
-        <v>483</v>
-      </c>
-      <c r="B252" t="s">
-        <v>541</v>
-      </c>
-      <c r="C252">
-        <v>2090</v>
-      </c>
-      <c r="D252" t="s">
-        <v>542</v>
-      </c>
-      <c r="E252" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="253" spans="1:5">
-      <c r="A253" t="s">
-        <v>483</v>
-      </c>
-      <c r="B253" t="s">
-        <v>543</v>
-      </c>
-      <c r="E253" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="254" spans="1:5">
-      <c r="A254" t="s">
-        <v>483</v>
-      </c>
-      <c r="B254" t="s">
-        <v>544</v>
-      </c>
-      <c r="E254" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5">
-      <c r="A255" t="s">
-        <v>483</v>
-      </c>
-      <c r="B255" t="s">
-        <v>545</v>
-      </c>
-      <c r="E255" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="256" spans="1:5">
-      <c r="A256" t="s">
-        <v>483</v>
-      </c>
-      <c r="B256" t="s">
-        <v>546</v>
-      </c>
-      <c r="E256" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5">
-      <c r="A257" t="s">
-        <v>483</v>
-      </c>
-      <c r="B257" t="s">
-        <v>547</v>
-      </c>
-      <c r="E257" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5">
-      <c r="A258" t="s">
-        <v>483</v>
-      </c>
-      <c r="B258" t="s">
-        <v>548</v>
-      </c>
-      <c r="C258">
-        <v>2388</v>
-      </c>
-      <c r="D258" t="s">
-        <v>549</v>
-      </c>
-      <c r="E258" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="259" spans="1:5">
-      <c r="A259" t="s">
-        <v>483</v>
-      </c>
-      <c r="B259" t="s">
-        <v>551</v>
-      </c>
-      <c r="E259" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="260" spans="1:5">
-      <c r="A260" t="s">
-        <v>483</v>
-      </c>
-      <c r="B260" t="s">
-        <v>552</v>
-      </c>
-      <c r="E260" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="261" spans="1:5">
-      <c r="A261" t="s">
-        <v>483</v>
-      </c>
-      <c r="B261" t="s">
-        <v>553</v>
-      </c>
-      <c r="E261" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="262" spans="1:5">
-      <c r="A262" t="s">
-        <v>483</v>
-      </c>
-      <c r="B262" t="s">
-        <v>554</v>
-      </c>
-      <c r="C262">
-        <v>108987</v>
-      </c>
-      <c r="D262" t="s">
-        <v>555</v>
-      </c>
-      <c r="E262" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="263" spans="1:5">
-      <c r="A263" t="s">
-        <v>483</v>
-      </c>
-      <c r="B263" t="s">
-        <v>557</v>
-      </c>
-      <c r="E263" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="264" spans="1:5">
-      <c r="A264" t="s">
-        <v>483</v>
-      </c>
-      <c r="B264" t="s">
-        <v>558</v>
-      </c>
-      <c r="C264">
-        <v>116688</v>
-      </c>
-      <c r="D264" t="s">
-        <v>559</v>
-      </c>
-      <c r="E264" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5">
-      <c r="A265" t="s">
-        <v>483</v>
-      </c>
-      <c r="B265" t="s">
-        <v>561</v>
-      </c>
-      <c r="C265">
-        <v>176628</v>
-      </c>
-      <c r="D265" t="s">
-        <v>562</v>
-      </c>
-      <c r="E265" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5">
-      <c r="A266" t="s">
-        <v>483</v>
-      </c>
-      <c r="B266" t="s">
-        <v>564</v>
-      </c>
-      <c r="C266">
-        <v>5241</v>
-      </c>
-      <c r="D266" t="s">
-        <v>565</v>
-      </c>
-      <c r="E266" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5">
-      <c r="A267" t="s">
-        <v>483</v>
-      </c>
-      <c r="B267" t="s">
-        <v>567</v>
-      </c>
-      <c r="E267" t="s">
-        <v>624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>